<commit_message>
string manipulation in python
</commit_message>
<xml_diff>
--- a/interview_prep_tracker 2025.xlsx
+++ b/interview_prep_tracker 2025.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JOHNPAUL\learning\learn-algorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3B7C36-BAAC-438F-9ABC-085D9DDC3C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A485F350-0A8D-4DAC-B261-45C541B7C9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="11440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LeetCode Tracker" sheetId="1" r:id="rId1"/>
-    <sheet name="System Design" sheetId="2" r:id="rId2"/>
-    <sheet name="Behavioral Prep" sheetId="3" r:id="rId3"/>
+    <sheet name="Basic Python Code" sheetId="5" r:id="rId2"/>
+    <sheet name="System Design" sheetId="2" r:id="rId3"/>
+    <sheet name="Behavioral Prep" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="370">
   <si>
     <t>Date</t>
   </si>
@@ -503,13 +504,1014 @@
   </si>
   <si>
     <t>Product of Array Except Self</t>
+  </si>
+  <si>
+    <t>1–20: String Manipulation</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Reverse every </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-character chunk of a string, dropping the last chunk if shorter than </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>k</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. Rotate a string to the left by </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> characters (manual shifting)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3. For each </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-char chunk, move its first character to the end</t>
+    </r>
+  </si>
+  <si>
+    <t>4. Remove all vowels from a string</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5. Count the number of palindromic substrings of length exactly </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>k</t>
+    </r>
+  </si>
+  <si>
+    <t>6. Replace each digit in a string with its English name (e.g., '1' → “one”)</t>
+  </si>
+  <si>
+    <t>7. Implement case inversion: lowercase → uppercase and vice versa</t>
+  </si>
+  <si>
+    <t>8. Compress a string by replacing runs (e.g., “aaabb” → “a3b2”)</t>
+  </si>
+  <si>
+    <t>9. Expand a compressed string (reverse of #8)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10. Group consecutive identical letters with their counts (produce </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>[('a',3), ('b',2), …]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>11. Check if one string is a rotation of another (manual search)</t>
+  </si>
+  <si>
+    <t>12. Find the longest run of identical characters</t>
+  </si>
+  <si>
+    <t>13. Remove all duplicate characters, preserving only their first occurrence</t>
+  </si>
+  <si>
+    <t>14. Merge two strings by alternating characters</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">15. Given a string, produce its zig-zag reading across </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> rows</t>
+    </r>
+  </si>
+  <si>
+    <t>16. Check if two strings are anagrams (manual letter counting)</t>
+  </si>
+  <si>
+    <r>
+      <t>17. Implement basic wildcard matching (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">=one char, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=any sequence)</t>
+    </r>
+  </si>
+  <si>
+    <t>18. Remove all characters that appear more than once</t>
+  </si>
+  <si>
+    <t>19. Reverse all words in a sentence (words are space-separated)</t>
+  </si>
+  <si>
+    <t>20. Capitalize the first letter of each sentence (detect sentence ends manually)</t>
+  </si>
+  <si>
+    <t>🔄 21–40: Numeric/String Hybrid</t>
+  </si>
+  <si>
+    <t>21. Convert a string of digits to integer (manually)</t>
+  </si>
+  <si>
+    <t>22. Integer to string conversion</t>
+  </si>
+  <si>
+    <t>23. Add two large numbers represented as strings</t>
+  </si>
+  <si>
+    <t>24. Multiply two large numbers represented as strings</t>
+  </si>
+  <si>
+    <t>25. Perform basic subtraction of large string-numbers</t>
+  </si>
+  <si>
+    <t>26. Validate a credit-card number using the Luhn algorithm</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">27. Format a 10-digit string as phone-number style: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>(xxx) xxx-xxxx</t>
+    </r>
+  </si>
+  <si>
+    <t>28. Convert a decimal string to binary string</t>
+  </si>
+  <si>
+    <t>29. Convert a binary string to decimal integer</t>
+  </si>
+  <si>
+    <t>30. Evaluate a simple arithmetic expression with + and – only</t>
+  </si>
+  <si>
+    <t>31. Check if a string-represented number is prime (trial division)</t>
+  </si>
+  <si>
+    <t>32. Compute factorial of a number without recursion</t>
+  </si>
+  <si>
+    <t>33. Reverse bits of an integer within a fixed bit‑width (e.g. 8 bits)</t>
+  </si>
+  <si>
+    <t>34. Count the number of 1-bits in a binary representation</t>
+  </si>
+  <si>
+    <t>35. Convert Roman numerals to integer</t>
+  </si>
+  <si>
+    <t>36. Convert integer to Roman numerals</t>
+  </si>
+  <si>
+    <t>37. Find greatest common divisor (GCD) using Euclid’s algorithm</t>
+  </si>
+  <si>
+    <t>38. Compute least common multiple (LCM) via GCD</t>
+  </si>
+  <si>
+    <t>39. Given a number, produce its digits in descending order</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">40. Generate the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>kth</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> permutation in numeric or character order manually</t>
+    </r>
+  </si>
+  <si>
+    <t>🔄 41–60: Array &amp; List Problems</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">41. Reverse every </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-element chunk in a list</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">42. Rotate a list right by </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>k</t>
+    </r>
+  </si>
+  <si>
+    <t>43. Left-pad a list with zeros to a target size</t>
+  </si>
+  <si>
+    <t>44. Run-length encode a list</t>
+  </si>
+  <si>
+    <t>45. Remove duplicates from an unsorted list in place</t>
+  </si>
+  <si>
+    <t>46. Segregate zeros and ones in a binary list</t>
+  </si>
+  <si>
+    <t>47. Sort a list of 0s, 1s, 2s (Dutch National Flag)</t>
+  </si>
+  <si>
+    <t>48. Merge two sorted lists</t>
+  </si>
+  <si>
+    <t>49. Implement merge for multiple sorted sublists (k-way merge)</t>
+  </si>
+  <si>
+    <t>50. Implement "two-sum" with O(n) memory</t>
+  </si>
+  <si>
+    <t>51. Move all occurrences of a particular value to the end</t>
+  </si>
+  <si>
+    <t>52. Given an array and target, find triplets summing to zero (only brute force)</t>
+  </si>
+  <si>
+    <t>53. Find contiguous subarray with max sum (Kadane’s algorithm, manual)</t>
+  </si>
+  <si>
+    <t>54. Remove all elements equal to a given value</t>
+  </si>
+  <si>
+    <t>55. Rotate a matrix by 90° clockwise (in-place with loops)</t>
+  </si>
+  <si>
+    <t>56. Transpose a matrix manually</t>
+  </si>
+  <si>
+    <t>57. Zero-out rows and columns in a matrix if any element is zero</t>
+  </si>
+  <si>
+    <t>58. Spiral order traversal of a matrix</t>
+  </si>
+  <si>
+    <t>59. Verify if a matrix is symmetrical (with loops)</t>
+  </si>
+  <si>
+    <t>60. Multiply two matrices</t>
+  </si>
+  <si>
+    <t>🔃 61–80: Linked-List Style (Using Arrays/Pointers)</t>
+  </si>
+  <si>
+    <t>61. Reverse a list (in place)</t>
+  </si>
+  <si>
+    <t>62. Detect loop in a “linked” list represented via index references</t>
+  </si>
+  <si>
+    <t>63. Find the middle element of a list</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">64. Remove the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>kth</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> element from the end</t>
+    </r>
+  </si>
+  <si>
+    <t>65. Merge two sorted lists</t>
+  </si>
+  <si>
+    <t>66. Partition list around a pivot value</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">67. Reverse nodes in blocks of size </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>k</t>
+    </r>
+  </si>
+  <si>
+    <t>68. Check if a list is a palindrome</t>
+  </si>
+  <si>
+    <t>69. Remove all occurrences of a value</t>
+  </si>
+  <si>
+    <t>70. Intersection of two “linked” lists (by index pointers)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">71. Reverse every alternate </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-element block</t>
+    </r>
+  </si>
+  <si>
+    <t>72. Swap pairs of elements</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">73. Rotate list right by </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> positions</t>
+    </r>
+  </si>
+  <si>
+    <t>74. Delete duplicates from a sorted list</t>
+  </si>
+  <si>
+    <t>75. Add two numbers represented as reversed linked lists (digit by digit)</t>
+  </si>
+  <si>
+    <t>76. Given separate files for head/tail pointers: implement pop/push</t>
+  </si>
+  <si>
+    <t>77. Flatten a nested list of lists (linked list style)</t>
+  </si>
+  <si>
+    <t>78. Convert array-to-struct (coalesce sensors data)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">79. Move last element to front iteratively </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> times</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">80. Split list into </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> equal parts (as evenly as possible)</t>
+    </r>
+  </si>
+  <si>
+    <t>📋 81–100: Mixed / Story-Based Patterns</t>
+  </si>
+  <si>
+    <t>81. Simulate a queue using two stacks (arrays)</t>
+  </si>
+  <si>
+    <t>82. Simulate a stack using two queues (arrays)</t>
+  </si>
+  <si>
+    <t>83. Implement a circular buffer (fixed-size queue)</t>
+  </si>
+  <si>
+    <t>84. Evaluate postfix (Reverse Polish) arithmetic expression</t>
+  </si>
+  <si>
+    <t>85. Convert infix expression (with +, –, *, /, parentheses) to postfix</t>
+  </si>
+  <si>
+    <t>86. Validate correct parenthesis matching (using manual stack)</t>
+  </si>
+  <si>
+    <t>87. In-order traversal of a binary tree (represented via dicts)</t>
+  </si>
+  <si>
+    <t>88. Pre-order traversal</t>
+  </si>
+  <si>
+    <t>89. Post-order traversal</t>
+  </si>
+  <si>
+    <t>90. Level-order (breadth-first) traversal</t>
+  </si>
+  <si>
+    <t>91. Serialize and deserialize a binary tree using arrays</t>
+  </si>
+  <si>
+    <t>92. Check if a binary tree is height-balanced</t>
+  </si>
+  <si>
+    <t>93. Calculate max depth of a binary tree</t>
+  </si>
+  <si>
+    <t>94. Check if a binary tree is symmetric</t>
+  </si>
+  <si>
+    <t>95. Find lowest common ancestor (LCA) of two nodes</t>
+  </si>
+  <si>
+    <t>96. Implement a simple hash map with open addressing</t>
+  </si>
+  <si>
+    <t>97. Implement a bloom filter (bit-array + k hashes)</t>
+  </si>
+  <si>
+    <t>98. Simulate LRU cache with fixed-size buffer</t>
+  </si>
+  <si>
+    <t>99. Perform topological sort on a DAG (manually)</t>
+  </si>
+  <si>
+    <t>100. Detect cycle in directed graph using DFS</t>
+  </si>
+  <si>
+    <t>✅ Beginner (1–30)</t>
+  </si>
+  <si>
+    <t>Print "Hello, World!"</t>
+  </si>
+  <si>
+    <t>Swap two variables.</t>
+  </si>
+  <si>
+    <t>Find the largest of three numbers.</t>
+  </si>
+  <si>
+    <t>Check if a number is even or odd.</t>
+  </si>
+  <si>
+    <t>Check if a number is prime.</t>
+  </si>
+  <si>
+    <t>Find the factorial of a number.</t>
+  </si>
+  <si>
+    <t>Generate the Fibonacci sequence.</t>
+  </si>
+  <si>
+    <t>Check if a string is a palindrome.</t>
+  </si>
+  <si>
+    <t>Count vowels and consonants in a string.</t>
+  </si>
+  <si>
+    <t>Reverse a number.</t>
+  </si>
+  <si>
+    <t>Sum of digits of a number.</t>
+  </si>
+  <si>
+    <t>Find ASCII value of a character.</t>
+  </si>
+  <si>
+    <t>Print all prime numbers in a range.</t>
+  </si>
+  <si>
+    <t>Find GCD of two numbers.</t>
+  </si>
+  <si>
+    <t>Find LCM of two numbers.</t>
+  </si>
+  <si>
+    <t>Check leap year.</t>
+  </si>
+  <si>
+    <t>Convert decimal to binary.</t>
+  </si>
+  <si>
+    <t>Convert binary to decimal.</t>
+  </si>
+  <si>
+    <t>Find the length of a string without using len().</t>
+  </si>
+  <si>
+    <t>Count occurrences of an element in a list.</t>
+  </si>
+  <si>
+    <t>Remove duplicates from a list.</t>
+  </si>
+  <si>
+    <t>Sort a list without using built-in methods.</t>
+  </si>
+  <si>
+    <t>Merge two sorted lists.</t>
+  </si>
+  <si>
+    <t>Find the second largest number in a list.</t>
+  </si>
+  <si>
+    <t>Check if a number is an Armstrong number.</t>
+  </si>
+  <si>
+    <t>Find the sum of elements in a list.</t>
+  </si>
+  <si>
+    <t>Reverse a list.</t>
+  </si>
+  <si>
+    <t>Create a multiplication table.</t>
+  </si>
+  <si>
+    <t>Calculate simple interest.</t>
+  </si>
+  <si>
+    <t>Generate a random number.</t>
+  </si>
+  <si>
+    <t>🔁 Intermediate (31–70)</t>
+  </si>
+  <si>
+    <t>Check if a string is an anagram.</t>
+  </si>
+  <si>
+    <t>Find all pairs in a list with a given sum.</t>
+  </si>
+  <si>
+    <t>Implement a stack using a list.</t>
+  </si>
+  <si>
+    <t>Implement a queue using a list.</t>
+  </si>
+  <si>
+    <t>Find the frequency of characters in a string.</t>
+  </si>
+  <si>
+    <t>Count the number of words in a string.</t>
+  </si>
+  <si>
+    <t>Check if a substring exists in a string.</t>
+  </si>
+  <si>
+    <t>Create a simple calculator using functions.</t>
+  </si>
+  <si>
+    <t>Implement binary search.</t>
+  </si>
+  <si>
+    <t>Implement linear search.</t>
+  </si>
+  <si>
+    <t>Recursive function to calculate power.</t>
+  </si>
+  <si>
+    <t>Convert Roman numeral to integer.</t>
+  </si>
+  <si>
+    <t>Convert integer to Roman numeral.</t>
+  </si>
+  <si>
+    <t>Find common elements in two lists.</t>
+  </si>
+  <si>
+    <t>Count number of lines, words, and characters in a file.</t>
+  </si>
+  <si>
+    <t>Read and write to a text file.</t>
+  </si>
+  <si>
+    <t>Remove punctuation from a string.</t>
+  </si>
+  <si>
+    <t>Check if two strings are isomorphic.</t>
+  </si>
+  <si>
+    <t>Implement bubble sort.</t>
+  </si>
+  <si>
+    <t>Implement selection sort.</t>
+  </si>
+  <si>
+    <t>Implement insertion sort.</t>
+  </si>
+  <si>
+    <t>Merge two dictionaries.</t>
+  </si>
+  <si>
+    <t>Find the most frequent element in a list.</t>
+  </si>
+  <si>
+    <t>Convert a list of tuples to a dictionary.</t>
+  </si>
+  <si>
+    <t>Flatten a nested list.</t>
+  </si>
+  <si>
+    <t>Print Pascal’s triangle.</t>
+  </si>
+  <si>
+    <t>Implement matrix multiplication.</t>
+  </si>
+  <si>
+    <t>Transpose a matrix.</t>
+  </si>
+  <si>
+    <t>Calculate sum of each row and column in a matrix.</t>
+  </si>
+  <si>
+    <t>Create a dictionary from two lists.</t>
+  </si>
+  <si>
+    <t>Find the longest word in a sentence.</t>
+  </si>
+  <si>
+    <t>Convert temperature from Celsius to Fahrenheit.</t>
+  </si>
+  <si>
+    <t>Check if a string contains only digits.</t>
+  </si>
+  <si>
+    <t>Calculate the power of a number using recursion.</t>
+  </si>
+  <si>
+    <t>Count the number of occurrences of a word in a file.</t>
+  </si>
+  <si>
+    <t>Find the largest and smallest number in a list.</t>
+  </si>
+  <si>
+    <t>Check if a number is a perfect number.</t>
+  </si>
+  <si>
+    <t>Find the sum of even numbers in a list.</t>
+  </si>
+  <si>
+    <t>Sort words in a sentence alphabetically.</t>
+  </si>
+  <si>
+    <t>Remove all whitespace from a string.</t>
+  </si>
+  <si>
+    <t>🚀 Advanced (71–100)</t>
+  </si>
+  <si>
+    <t>Find the longest common prefix among a list of strings.</t>
+  </si>
+  <si>
+    <t>Implement a simple phone book using a dictionary.</t>
+  </si>
+  <si>
+    <t>Implement quicksort.</t>
+  </si>
+  <si>
+    <t>Implement mergesort.</t>
+  </si>
+  <si>
+    <t>Implement a linked list.</t>
+  </si>
+  <si>
+    <t>Detect a cycle in a linked list.</t>
+  </si>
+  <si>
+    <t>Implement a binary search tree.</t>
+  </si>
+  <si>
+    <t>Find the height of a binary tree.</t>
+  </si>
+  <si>
+    <t>Check if two binary trees are identical.</t>
+  </si>
+  <si>
+    <t>Find the lowest common ancestor in a binary tree.</t>
+  </si>
+  <si>
+    <t>Implement depth-first search (DFS).</t>
+  </si>
+  <si>
+    <t>Implement breadth-first search (BFS).</t>
+  </si>
+  <si>
+    <t>Implement a graph using an adjacency list.</t>
+  </si>
+  <si>
+    <t>Check if a graph is connected.</t>
+  </si>
+  <si>
+    <t>Perform topological sort of a graph.</t>
+  </si>
+  <si>
+    <t>Implement Dijkstra's shortest path algorithm.</t>
+  </si>
+  <si>
+    <t>Find all permutations of a string.</t>
+  </si>
+  <si>
+    <t>Find all subsets of a set.</t>
+  </si>
+  <si>
+    <t>Solve the N-Queens problem.</t>
+  </si>
+  <si>
+    <t>Solve the Tower of Hanoi problem.</t>
+  </si>
+  <si>
+    <t>Implement a caching system (LRU cache).</t>
+  </si>
+  <si>
+    <t>Implement a decorator.</t>
+  </si>
+  <si>
+    <t>Implement a context manager using with.</t>
+  </si>
+  <si>
+    <t>Multithreaded program to print numbers alternately.</t>
+  </si>
+  <si>
+    <t>Use map(), filter(), and reduce() with lambdas.</t>
+  </si>
+  <si>
+    <t>Create and use a custom Python package.</t>
+  </si>
+  <si>
+    <t>Parse JSON data from a file.</t>
+  </si>
+  <si>
+    <t>Connect to an SQLite database and perform CRUD operations.</t>
+  </si>
+  <si>
+    <t>Use regular expressions to extract email addresses.</t>
+  </si>
+  <si>
+    <t>Measure execution time of a function.</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Need to check</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -532,8 +1534,29 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -543,6 +1566,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -607,7 +1642,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -628,6 +1663,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -935,22 +1985,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H154"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="B20" sqref="B14:B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="9.453125" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.90625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="13.08984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.81640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="15.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="67.90625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="67.81640625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -976,7 +2026,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8">
       <c r="A2" s="4">
         <v>45755</v>
       </c>
@@ -1002,7 +2052,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8">
       <c r="A3" s="8">
         <v>45776</v>
       </c>
@@ -1028,7 +2078,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8">
       <c r="A4" s="8"/>
       <c r="B4" s="6" t="s">
         <v>41</v>
@@ -1043,7 +2093,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8">
       <c r="B5" s="6" t="s">
         <v>41</v>
       </c>
@@ -1057,7 +2107,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8">
       <c r="A6" s="9"/>
       <c r="B6" s="6" t="s">
         <v>41</v>
@@ -1067,7 +2117,7 @@
       </c>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8">
       <c r="A7" s="9"/>
       <c r="B7" s="6" t="s">
         <v>41</v>
@@ -1077,7 +2127,7 @@
       </c>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8">
       <c r="A8" s="9"/>
       <c r="B8" s="6" t="s">
         <v>41</v>
@@ -1087,7 +2137,7 @@
       </c>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8">
       <c r="A9" s="9"/>
       <c r="B9" s="6" t="s">
         <v>41</v>
@@ -1097,7 +2147,7 @@
       </c>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8">
       <c r="A10" s="9"/>
       <c r="B10" s="6" t="s">
         <v>41</v>
@@ -1107,7 +2157,7 @@
       </c>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8">
       <c r="A11" s="9"/>
       <c r="B11" s="6" t="s">
         <v>41</v>
@@ -1117,7 +2167,7 @@
       </c>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8">
       <c r="A12" s="9"/>
       <c r="B12" s="6" t="s">
         <v>41</v>
@@ -1127,7 +2177,7 @@
       </c>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8">
       <c r="A13" s="9"/>
       <c r="B13" s="6" t="s">
         <v>41</v>
@@ -1137,7 +2187,7 @@
       </c>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8">
       <c r="A14" s="9"/>
       <c r="B14" s="6" t="s">
         <v>48</v>
@@ -1147,7 +2197,7 @@
       </c>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8">
       <c r="A15" s="9"/>
       <c r="B15" s="6" t="s">
         <v>48</v>
@@ -1157,7 +2207,7 @@
       </c>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8">
       <c r="A16" s="9"/>
       <c r="B16" s="6" t="s">
         <v>48</v>
@@ -1167,7 +2217,7 @@
       </c>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8">
       <c r="A17" s="9"/>
       <c r="B17" s="6" t="s">
         <v>48</v>
@@ -1177,7 +2227,7 @@
       </c>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8">
       <c r="A18" s="9"/>
       <c r="B18" s="6" t="s">
         <v>48</v>
@@ -1187,7 +2237,7 @@
       </c>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8">
       <c r="A19" s="9"/>
       <c r="B19" s="6" t="s">
         <v>48</v>
@@ -1197,7 +2247,7 @@
       </c>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8">
       <c r="A20" s="9"/>
       <c r="B20" s="6" t="s">
         <v>48</v>
@@ -1207,7 +2257,7 @@
       </c>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8">
       <c r="A21" s="10"/>
       <c r="B21" s="6" t="s">
         <v>48</v>
@@ -1219,7 +2269,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8">
       <c r="A22" s="10"/>
       <c r="B22" s="6" t="s">
         <v>48</v>
@@ -1231,7 +2281,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8">
       <c r="A23" s="10"/>
       <c r="B23" s="6" t="s">
         <v>48</v>
@@ -1243,7 +2293,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8">
       <c r="A24" s="10"/>
       <c r="B24" s="6" t="s">
         <v>48</v>
@@ -1255,7 +2305,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8">
       <c r="A25" s="10"/>
       <c r="B25" s="6" t="s">
         <v>55</v>
@@ -1267,7 +2317,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8">
       <c r="A26" s="10"/>
       <c r="B26" s="6" t="s">
         <v>55</v>
@@ -1279,7 +2329,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8">
       <c r="A27" s="11"/>
       <c r="B27" s="6" t="s">
         <v>55</v>
@@ -1291,7 +2341,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8">
       <c r="B28" s="6" t="s">
         <v>55</v>
       </c>
@@ -1302,7 +2352,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8">
       <c r="B29" s="6" t="s">
         <v>55</v>
       </c>
@@ -1313,7 +2363,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8">
       <c r="B30" s="6" t="s">
         <v>55</v>
       </c>
@@ -1324,7 +2374,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8">
       <c r="B31" s="6" t="s">
         <v>55</v>
       </c>
@@ -1335,7 +2385,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8">
       <c r="B32" s="6" t="s">
         <v>55</v>
       </c>
@@ -1346,7 +2396,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:8">
       <c r="B33" s="6" t="s">
         <v>55</v>
       </c>
@@ -1357,7 +2407,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:8">
       <c r="B34" s="6" t="s">
         <v>55</v>
       </c>
@@ -1368,7 +2418,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:8">
       <c r="B35" s="6" t="s">
         <v>62</v>
       </c>
@@ -1379,7 +2429,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:8">
       <c r="B36" s="6" t="s">
         <v>62</v>
       </c>
@@ -1390,7 +2440,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:8">
       <c r="B37" s="6" t="s">
         <v>62</v>
       </c>
@@ -1401,7 +2451,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:8">
       <c r="B38" s="6" t="s">
         <v>62</v>
       </c>
@@ -1412,7 +2462,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:8">
       <c r="B39" s="6" t="s">
         <v>62</v>
       </c>
@@ -1423,7 +2473,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:8">
       <c r="B40" s="6" t="s">
         <v>62</v>
       </c>
@@ -1434,7 +2484,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:8">
       <c r="B41" s="6" t="s">
         <v>62</v>
       </c>
@@ -1445,7 +2495,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:8">
       <c r="B42" s="6" t="s">
         <v>62</v>
       </c>
@@ -1456,7 +2506,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:8">
       <c r="B43" s="6" t="s">
         <v>62</v>
       </c>
@@ -1467,7 +2517,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:8">
       <c r="B44" s="6" t="s">
         <v>62</v>
       </c>
@@ -1478,7 +2528,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:8">
       <c r="B45" s="6" t="s">
         <v>69</v>
       </c>
@@ -1489,7 +2539,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:8">
       <c r="B46" s="6" t="s">
         <v>69</v>
       </c>
@@ -1500,7 +2550,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:8">
       <c r="B47" s="6" t="s">
         <v>69</v>
       </c>
@@ -1511,7 +2561,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:8">
       <c r="B48" s="6" t="s">
         <v>69</v>
       </c>
@@ -1522,7 +2572,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:8">
       <c r="B49" s="6" t="s">
         <v>69</v>
       </c>
@@ -1533,7 +2583,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:8">
       <c r="B50" s="6" t="s">
         <v>69</v>
       </c>
@@ -1544,7 +2594,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:8">
       <c r="B51" s="6" t="s">
         <v>69</v>
       </c>
@@ -1555,7 +2605,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:8">
       <c r="B52" s="6" t="s">
         <v>69</v>
       </c>
@@ -1566,7 +2616,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:8">
       <c r="B53" s="6" t="s">
         <v>69</v>
       </c>
@@ -1577,7 +2627,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:8">
       <c r="B54" s="6" t="s">
         <v>69</v>
       </c>
@@ -1588,7 +2638,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:8">
       <c r="B55" s="6" t="s">
         <v>76</v>
       </c>
@@ -1599,7 +2649,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:8">
       <c r="B56" s="6" t="s">
         <v>76</v>
       </c>
@@ -1610,7 +2660,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:8">
       <c r="B57" s="6" t="s">
         <v>76</v>
       </c>
@@ -1621,7 +2671,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:8">
       <c r="B58" s="6" t="s">
         <v>76</v>
       </c>
@@ -1632,7 +2682,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:8">
       <c r="B59" s="6" t="s">
         <v>76</v>
       </c>
@@ -1643,7 +2693,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:8">
       <c r="B60" s="6" t="s">
         <v>76</v>
       </c>
@@ -1654,7 +2704,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:8">
       <c r="B61" s="6" t="s">
         <v>76</v>
       </c>
@@ -1665,7 +2715,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:8">
       <c r="B62" s="6" t="s">
         <v>76</v>
       </c>
@@ -1676,7 +2726,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:8">
       <c r="B63" s="6" t="s">
         <v>76</v>
       </c>
@@ -1687,7 +2737,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:8">
       <c r="B64" s="6" t="s">
         <v>76</v>
       </c>
@@ -1698,7 +2748,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:8">
       <c r="B65" s="6" t="s">
         <v>83</v>
       </c>
@@ -1709,7 +2759,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:8">
       <c r="B66" s="6" t="s">
         <v>83</v>
       </c>
@@ -1720,7 +2770,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:8">
       <c r="B67" s="6" t="s">
         <v>83</v>
       </c>
@@ -1731,7 +2781,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:8">
       <c r="B68" s="6" t="s">
         <v>83</v>
       </c>
@@ -1742,7 +2792,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:8">
       <c r="B69" s="6" t="s">
         <v>83</v>
       </c>
@@ -1753,7 +2803,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:8">
       <c r="B70" s="6" t="s">
         <v>83</v>
       </c>
@@ -1764,7 +2814,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:8">
       <c r="B71" s="6" t="s">
         <v>83</v>
       </c>
@@ -1775,7 +2825,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:8">
       <c r="B72" s="6" t="s">
         <v>83</v>
       </c>
@@ -1786,7 +2836,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:8">
       <c r="B73" s="6" t="s">
         <v>83</v>
       </c>
@@ -1797,7 +2847,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:8">
       <c r="B74" s="6" t="s">
         <v>83</v>
       </c>
@@ -1808,7 +2858,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:8">
       <c r="B75" s="6" t="s">
         <v>90</v>
       </c>
@@ -1819,7 +2869,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:8">
       <c r="B76" s="6" t="s">
         <v>90</v>
       </c>
@@ -1830,7 +2880,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:8">
       <c r="B77" s="6" t="s">
         <v>90</v>
       </c>
@@ -1841,7 +2891,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:8">
       <c r="B78" s="6" t="s">
         <v>90</v>
       </c>
@@ -1852,7 +2902,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:8">
       <c r="B79" s="6" t="s">
         <v>90</v>
       </c>
@@ -1863,7 +2913,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:8">
       <c r="B80" s="6" t="s">
         <v>90</v>
       </c>
@@ -1874,7 +2924,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:8">
       <c r="B81" s="6" t="s">
         <v>90</v>
       </c>
@@ -1885,7 +2935,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:8">
       <c r="B82" s="6" t="s">
         <v>90</v>
       </c>
@@ -1896,7 +2946,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:8">
       <c r="B83" s="6" t="s">
         <v>90</v>
       </c>
@@ -1907,7 +2957,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:8">
       <c r="B84" s="6" t="s">
         <v>90</v>
       </c>
@@ -1918,7 +2968,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:8">
       <c r="B85" s="6" t="s">
         <v>97</v>
       </c>
@@ -1929,7 +2979,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:8">
       <c r="B86" s="6" t="s">
         <v>97</v>
       </c>
@@ -1940,7 +2990,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:8">
       <c r="B87" s="6" t="s">
         <v>97</v>
       </c>
@@ -1951,7 +3001,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:8">
       <c r="B88" s="6" t="s">
         <v>97</v>
       </c>
@@ -1962,7 +3012,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:8">
       <c r="B89" s="6" t="s">
         <v>97</v>
       </c>
@@ -1973,7 +3023,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:8">
       <c r="B90" s="6" t="s">
         <v>97</v>
       </c>
@@ -1984,7 +3034,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:8">
       <c r="B91" s="6" t="s">
         <v>97</v>
       </c>
@@ -1995,7 +3045,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:8">
       <c r="B92" s="6" t="s">
         <v>97</v>
       </c>
@@ -2006,7 +3056,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:8">
       <c r="B93" s="6" t="s">
         <v>97</v>
       </c>
@@ -2017,7 +3067,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:8">
       <c r="B94" s="6" t="s">
         <v>97</v>
       </c>
@@ -2028,7 +3078,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:8">
       <c r="B95" s="6" t="s">
         <v>104</v>
       </c>
@@ -2039,7 +3089,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:8">
       <c r="B96" s="6" t="s">
         <v>104</v>
       </c>
@@ -2050,7 +3100,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:8">
       <c r="B97" s="6" t="s">
         <v>104</v>
       </c>
@@ -2061,7 +3111,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:8">
       <c r="B98" s="6" t="s">
         <v>104</v>
       </c>
@@ -2072,7 +3122,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:8">
       <c r="B99" s="6" t="s">
         <v>104</v>
       </c>
@@ -2083,7 +3133,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:8">
       <c r="B100" s="6" t="s">
         <v>104</v>
       </c>
@@ -2094,7 +3144,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:8">
       <c r="B101" s="6" t="s">
         <v>104</v>
       </c>
@@ -2105,7 +3155,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:8">
       <c r="B102" s="6" t="s">
         <v>104</v>
       </c>
@@ -2116,7 +3166,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:8">
       <c r="B103" s="6" t="s">
         <v>104</v>
       </c>
@@ -2127,7 +3177,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="104" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:8">
       <c r="B104" s="6" t="s">
         <v>104</v>
       </c>
@@ -2138,7 +3188,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:8">
       <c r="B105" s="6" t="s">
         <v>111</v>
       </c>
@@ -2149,7 +3199,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:8">
       <c r="B106" s="6" t="s">
         <v>111</v>
       </c>
@@ -2160,7 +3210,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="107" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:8">
       <c r="B107" s="6" t="s">
         <v>111</v>
       </c>
@@ -2171,7 +3221,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:8">
       <c r="B108" s="6" t="s">
         <v>111</v>
       </c>
@@ -2182,7 +3232,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="109" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:8">
       <c r="B109" s="6" t="s">
         <v>111</v>
       </c>
@@ -2193,7 +3243,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="110" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:8">
       <c r="B110" s="6" t="s">
         <v>111</v>
       </c>
@@ -2204,7 +3254,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="111" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:8">
       <c r="B111" s="6" t="s">
         <v>111</v>
       </c>
@@ -2215,7 +3265,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="112" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:8">
       <c r="B112" s="6" t="s">
         <v>111</v>
       </c>
@@ -2226,7 +3276,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="113" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:8">
       <c r="B113" s="6" t="s">
         <v>111</v>
       </c>
@@ -2237,7 +3287,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="114" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:8">
       <c r="B114" s="6" t="s">
         <v>111</v>
       </c>
@@ -2248,7 +3298,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:8">
       <c r="B115" s="6" t="s">
         <v>118</v>
       </c>
@@ -2259,7 +3309,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="116" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:8">
       <c r="B116" s="6" t="s">
         <v>118</v>
       </c>
@@ -2270,7 +3320,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="117" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:8">
       <c r="B117" s="6" t="s">
         <v>118</v>
       </c>
@@ -2281,7 +3331,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="118" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:8">
       <c r="B118" s="6" t="s">
         <v>118</v>
       </c>
@@ -2292,7 +3342,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="119" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:8">
       <c r="B119" s="6" t="s">
         <v>118</v>
       </c>
@@ -2303,7 +3353,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="120" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:8">
       <c r="B120" s="6" t="s">
         <v>118</v>
       </c>
@@ -2314,7 +3364,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="121" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:8">
       <c r="B121" s="6" t="s">
         <v>118</v>
       </c>
@@ -2325,7 +3375,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:8">
       <c r="B122" s="6" t="s">
         <v>118</v>
       </c>
@@ -2336,7 +3386,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="123" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:8">
       <c r="B123" s="6" t="s">
         <v>118</v>
       </c>
@@ -2347,7 +3397,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="124" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:8">
       <c r="B124" s="6" t="s">
         <v>118</v>
       </c>
@@ -2358,7 +3408,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="125" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:8">
       <c r="B125" s="6" t="s">
         <v>125</v>
       </c>
@@ -2369,7 +3419,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="126" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:8">
       <c r="B126" s="6" t="s">
         <v>125</v>
       </c>
@@ -2380,7 +3430,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="127" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:8">
       <c r="B127" s="6" t="s">
         <v>125</v>
       </c>
@@ -2391,7 +3441,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="128" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:8">
       <c r="B128" s="6" t="s">
         <v>125</v>
       </c>
@@ -2402,7 +3452,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:8">
       <c r="B129" s="6" t="s">
         <v>125</v>
       </c>
@@ -2413,7 +3463,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="130" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:8">
       <c r="B130" s="6" t="s">
         <v>125</v>
       </c>
@@ -2424,7 +3474,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:8">
       <c r="B131" s="6" t="s">
         <v>125</v>
       </c>
@@ -2435,7 +3485,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="132" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:8">
       <c r="B132" s="6" t="s">
         <v>125</v>
       </c>
@@ -2446,7 +3496,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="133" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:8">
       <c r="B133" s="6" t="s">
         <v>125</v>
       </c>
@@ -2457,7 +3507,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="134" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:8">
       <c r="B134" s="6" t="s">
         <v>125</v>
       </c>
@@ -2468,7 +3518,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="135" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:8">
       <c r="B135" s="6" t="s">
         <v>130</v>
       </c>
@@ -2479,7 +3529,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="136" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:8">
       <c r="B136" s="6" t="s">
         <v>130</v>
       </c>
@@ -2490,7 +3540,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="137" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:8">
       <c r="B137" s="6" t="s">
         <v>130</v>
       </c>
@@ -2501,7 +3551,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:8">
       <c r="B138" s="6" t="s">
         <v>130</v>
       </c>
@@ -2512,7 +3562,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="139" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:8">
       <c r="B139" s="6" t="s">
         <v>130</v>
       </c>
@@ -2523,7 +3573,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="140" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:8">
       <c r="B140" s="6" t="s">
         <v>130</v>
       </c>
@@ -2534,7 +3584,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="141" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:8">
       <c r="B141" s="6" t="s">
         <v>130</v>
       </c>
@@ -2545,7 +3595,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="142" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:8">
       <c r="B142" s="6" t="s">
         <v>130</v>
       </c>
@@ -2556,7 +3606,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="143" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:8">
       <c r="B143" s="6" t="s">
         <v>130</v>
       </c>
@@ -2567,7 +3617,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="144" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:8">
       <c r="B144" s="6" t="s">
         <v>130</v>
       </c>
@@ -2578,7 +3628,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="145" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:8">
       <c r="B145" s="6" t="s">
         <v>137</v>
       </c>
@@ -2589,7 +3639,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="146" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:8">
       <c r="B146" s="6" t="s">
         <v>137</v>
       </c>
@@ -2600,7 +3650,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="147" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:8">
       <c r="B147" s="6" t="s">
         <v>137</v>
       </c>
@@ -2611,7 +3661,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="148" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="148" spans="2:8">
       <c r="B148" s="6" t="s">
         <v>137</v>
       </c>
@@ -2622,7 +3672,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="149" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:8">
       <c r="B149" s="6" t="s">
         <v>137</v>
       </c>
@@ -2633,7 +3683,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="150" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="150" spans="2:8">
       <c r="B150" s="6" t="s">
         <v>137</v>
       </c>
@@ -2644,7 +3694,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="151" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="151" spans="2:8">
       <c r="B151" s="6" t="s">
         <v>137</v>
       </c>
@@ -2655,7 +3705,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="152" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:8">
       <c r="B152" s="6" t="s">
         <v>137</v>
       </c>
@@ -2666,7 +3716,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="153" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="153" spans="2:8">
       <c r="B153" s="6" t="s">
         <v>137</v>
       </c>
@@ -2677,7 +3727,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="154" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="154" spans="2:8">
       <c r="B154" s="6" t="s">
         <v>137</v>
       </c>
@@ -2834,16 +3884,1158 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C80EF47-4416-4B22-BDFD-DF2F4A2C465A}">
+  <dimension ref="A1:C209"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="81.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18" customHeight="1">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="6"/>
+      <c r="B2" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="8">
+        <v>45848</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="8">
+        <v>45849</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="8">
+        <v>45852</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="8">
+        <v>45855</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="8">
+        <v>45855</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="8">
+        <v>45858</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="8">
+        <v>45859</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="8">
+        <v>45859</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="8">
+        <v>45860</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="8"/>
+      <c r="B12" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="8">
+        <v>45866</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="8">
+        <v>45867</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="8">
+        <v>45867</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="8"/>
+      <c r="B16" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="8">
+        <v>45867</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="8">
+        <v>45868</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="8">
+        <v>45868</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="6"/>
+      <c r="B20" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="6"/>
+      <c r="B21" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="1:3" ht="18" customHeight="1">
+      <c r="B22" s="12" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="B23" s="13" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="B24" s="13" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="B25" s="13" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="B26" s="13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="B27" s="13" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="B28" s="13" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="B29" s="13" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="B30" s="13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="B31" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="B32" s="13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="13" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="13" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="13" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="13" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" s="13" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" s="13" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" s="13" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" s="13" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" ht="18" customHeight="1">
+      <c r="B43" s="12" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2">
+      <c r="B45" s="13" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" s="13" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" s="13" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2">
+      <c r="B48" s="13" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" s="13" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" s="13" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51" s="13" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52" s="13" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53" s="13" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2">
+      <c r="B54" s="13" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2">
+      <c r="B55" s="13" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2">
+      <c r="B56" s="13" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2">
+      <c r="B57" s="13" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2">
+      <c r="B58" s="13" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2">
+      <c r="B59" s="13" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2">
+      <c r="B60" s="13" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2">
+      <c r="B61" s="13" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2">
+      <c r="B62" s="13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2">
+      <c r="B63" s="13" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" ht="18" customHeight="1">
+      <c r="B64" s="12" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65" s="13" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2">
+      <c r="B66" s="13" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2">
+      <c r="B67" s="13" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2">
+      <c r="B68" s="13" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2">
+      <c r="B69" s="13" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2">
+      <c r="B70" s="13" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2">
+      <c r="B71" s="13" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2">
+      <c r="B72" s="13" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2">
+      <c r="B73" s="13" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2">
+      <c r="B74" s="13" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2">
+      <c r="B75" s="13" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2">
+      <c r="B76" s="13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2">
+      <c r="B77" s="13" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2">
+      <c r="B78" s="13" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2">
+      <c r="B79" s="13" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2">
+      <c r="B80" s="13" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2">
+      <c r="B81" s="13" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2">
+      <c r="B82" s="13" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2">
+      <c r="B83" s="13" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2">
+      <c r="B84" s="13" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" ht="18" customHeight="1">
+      <c r="B85" s="12" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2">
+      <c r="B86" s="13" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2">
+      <c r="B87" s="13" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2">
+      <c r="B88" s="13" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2">
+      <c r="B89" s="13" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2">
+      <c r="B90" s="13" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2">
+      <c r="B91" s="13" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2">
+      <c r="B92" s="13" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2">
+      <c r="B93" s="13" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2">
+      <c r="B94" s="13" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2">
+      <c r="B95" s="13" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2">
+      <c r="B96" s="13" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2">
+      <c r="B97" s="13" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2">
+      <c r="B98" s="13" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2">
+      <c r="B99" s="13" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2">
+      <c r="B100" s="13" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2">
+      <c r="B101" s="13" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2">
+      <c r="B102" s="13" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2">
+      <c r="B103" s="13" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2">
+      <c r="B104" s="13" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2">
+      <c r="B105" s="13" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2">
+      <c r="B106" s="13"/>
+    </row>
+    <row r="107" spans="2:2">
+      <c r="B107" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2">
+      <c r="B108" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2">
+      <c r="B109" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2">
+      <c r="B110" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2">
+      <c r="B111" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="112" spans="2:2">
+      <c r="B112" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2">
+      <c r="B113" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2">
+      <c r="B114" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="115" spans="2:2">
+      <c r="B115" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2">
+      <c r="B116" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="117" spans="2:2">
+      <c r="B117" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2">
+      <c r="B118" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2">
+      <c r="B119" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2">
+      <c r="B120" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2">
+      <c r="B121" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2">
+      <c r="B122" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="123" spans="2:2">
+      <c r="B123" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2">
+      <c r="B124" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="125" spans="2:2">
+      <c r="B125" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="126" spans="2:2">
+      <c r="B126" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="127" spans="2:2">
+      <c r="B127" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="128" spans="2:2">
+      <c r="B128" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="129" spans="2:2">
+      <c r="B129" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="130" spans="2:2">
+      <c r="B130" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2">
+      <c r="B131" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="132" spans="2:2">
+      <c r="B132" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="133" spans="2:2">
+      <c r="B133" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="134" spans="2:2">
+      <c r="B134" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2">
+      <c r="B135" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="136" spans="2:2">
+      <c r="B136" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2">
+      <c r="B137" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="138" spans="2:2">
+      <c r="B138" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="139" spans="2:2">
+      <c r="B139" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="140" spans="2:2">
+      <c r="B140" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="141" spans="2:2">
+      <c r="B141" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="142" spans="2:2">
+      <c r="B142" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="143" spans="2:2">
+      <c r="B143" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="144" spans="2:2">
+      <c r="B144" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="145" spans="2:2">
+      <c r="B145" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="146" spans="2:2">
+      <c r="B146" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="147" spans="2:2">
+      <c r="B147" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="148" spans="2:2">
+      <c r="B148" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="149" spans="2:2">
+      <c r="B149" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="150" spans="2:2">
+      <c r="B150" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="151" spans="2:2">
+      <c r="B151" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="152" spans="2:2">
+      <c r="B152" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="153" spans="2:2">
+      <c r="B153" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="154" spans="2:2">
+      <c r="B154" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="155" spans="2:2">
+      <c r="B155" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="156" spans="2:2">
+      <c r="B156" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="157" spans="2:2">
+      <c r="B157" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="158" spans="2:2">
+      <c r="B158" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="159" spans="2:2">
+      <c r="B159" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="160" spans="2:2">
+      <c r="B160" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="161" spans="2:2">
+      <c r="B161" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="162" spans="2:2">
+      <c r="B162" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="163" spans="2:2">
+      <c r="B163" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="164" spans="2:2">
+      <c r="B164" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="165" spans="2:2">
+      <c r="B165" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="166" spans="2:2">
+      <c r="B166" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="167" spans="2:2">
+      <c r="B167" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="168" spans="2:2">
+      <c r="B168" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="169" spans="2:2">
+      <c r="B169" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="170" spans="2:2">
+      <c r="B170" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="171" spans="2:2">
+      <c r="B171" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="172" spans="2:2">
+      <c r="B172" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="173" spans="2:2">
+      <c r="B173" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="174" spans="2:2">
+      <c r="B174" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="175" spans="2:2">
+      <c r="B175" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="176" spans="2:2">
+      <c r="B176" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="177" spans="2:2">
+      <c r="B177" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="178" spans="2:2">
+      <c r="B178" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="179" spans="2:2">
+      <c r="B179" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="180" spans="2:2">
+      <c r="B180" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="181" spans="2:2">
+      <c r="B181" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="182" spans="2:2">
+      <c r="B182" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="183" spans="2:2">
+      <c r="B183" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="184" spans="2:2">
+      <c r="B184" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="185" spans="2:2">
+      <c r="B185" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="186" spans="2:2">
+      <c r="B186" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="187" spans="2:2">
+      <c r="B187" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="188" spans="2:2">
+      <c r="B188" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="189" spans="2:2">
+      <c r="B189" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="190" spans="2:2">
+      <c r="B190" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="191" spans="2:2">
+      <c r="B191" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="192" spans="2:2">
+      <c r="B192" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="193" spans="2:2">
+      <c r="B193" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="194" spans="2:2">
+      <c r="B194" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="195" spans="2:2">
+      <c r="B195" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="196" spans="2:2">
+      <c r="B196" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="197" spans="2:2">
+      <c r="B197" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="198" spans="2:2">
+      <c r="B198" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="199" spans="2:2">
+      <c r="B199" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="200" spans="2:2">
+      <c r="B200" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="201" spans="2:2">
+      <c r="B201" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="202" spans="2:2">
+      <c r="B202" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="203" spans="2:2">
+      <c r="B203" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="204" spans="2:2">
+      <c r="B204" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="205" spans="2:2">
+      <c r="B205" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="206" spans="2:2">
+      <c r="B206" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="207" spans="2:2">
+      <c r="B207" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="208" spans="2:2">
+      <c r="B208" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="209" spans="2:2">
+      <c r="B209" t="s">
+        <v>367</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2854,7 +5046,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2865,7 +5057,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2876,7 +5068,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -2887,7 +5079,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2898,7 +5090,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -2921,15 +5113,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -2940,7 +5132,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -2951,7 +5143,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -2962,7 +5154,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -2973,7 +5165,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -2984,7 +5176,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
group all python into notebook.
</commit_message>
<xml_diff>
--- a/interview_prep_tracker 2025.xlsx
+++ b/interview_prep_tracker 2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JOHNPAUL\learning\learn-algorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B482B68-9038-42E2-8316-F9612588EFE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45023A22-E048-4B60-9C7E-526FFD81E325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="371">
   <si>
     <t>Date</t>
   </si>
@@ -1505,6 +1505,9 @@
   </si>
   <si>
     <t>Need to check</t>
+  </si>
+  <si>
+    <t>08/08/20255</t>
   </si>
 </sst>
 </file>
@@ -3887,8 +3890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C80EF47-4416-4B22-BDFD-DF2F4A2C465A}">
   <dimension ref="A1:C209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4068,14 +4071,18 @@
       <c r="C19" s="6"/>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="6"/>
+      <c r="A20" s="8">
+        <v>45875</v>
+      </c>
       <c r="B20" s="15" t="s">
         <v>179</v>
       </c>
       <c r="C20" s="6"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="6"/>
+      <c r="A21" s="8">
+        <v>45875</v>
+      </c>
       <c r="B21" s="15" t="s">
         <v>180</v>
       </c>
@@ -4087,6 +4094,9 @@
       </c>
     </row>
     <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>370</v>
+      </c>
       <c r="B23" s="13" t="s">
         <v>182</v>
       </c>

</xml_diff>